<commit_message>
update CustomerActivity Báo cáo hoạt động khách hàng
</commit_message>
<xml_diff>
--- a/CMS/wwwroot/Templates/Excels/Reports/CustomerActivityTemplate.xlsx
+++ b/CMS/wwwroot/Templates/Excels/Reports/CustomerActivityTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vets\PRU-Gift\cms\CMS\wwwroot\Templates\Excels\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daiichi\cms\CMS\wwwroot\Templates\Excels\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC94E18-A8F8-46A7-AF05-A67283A8B6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E25D6E-A386-4B1D-985A-0373ED0D8250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BA19E4D-8276-4ADD-8E60-EDF41859A0D1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ListData">Sheet1!$B$11:$F$12</definedName>
+    <definedName name="ListCustomerType">Sheet1!$B$5:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Báo cáo hoạt động khách hàng</t>
   </si>
@@ -47,55 +47,13 @@
     <t>Tổng hợp</t>
   </si>
   <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Tên khách hàng</t>
-  </si>
-  <si>
-    <t>ID Khách hàng</t>
-  </si>
-  <si>
-    <t>Phòng ban</t>
-  </si>
-  <si>
-    <t>Thời gian hoạt động</t>
-  </si>
-  <si>
-    <t>Chi tiết khách hàng</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>{{item.FullName}}</t>
-  </si>
-  <si>
-    <t>{{item.Username}}</t>
-  </si>
-  <si>
-    <t>{{item.Org}}</t>
-  </si>
-  <si>
-    <t>{{item.ActiveTime}}</t>
-  </si>
-  <si>
-    <t>{{Org}}</t>
-  </si>
-  <si>
-    <t>{{Staff}}</t>
-  </si>
-  <si>
-    <t>{{GA}}</t>
-  </si>
-  <si>
     <t>Từ ngày {{From}} đến ngày {{To}}</t>
   </si>
   <si>
-    <t>{{index+1}}</t>
+    <t>{{item.Name}}</t>
+  </si>
+  <si>
+    <t>{{item.Value}}</t>
   </si>
 </sst>
 </file>
@@ -185,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -206,25 +164,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,24 +492,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCD9E90-56C8-4BF3-808C-C39CCA88D7A6}">
-  <dimension ref="B1:AD12"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="10.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
@@ -565,15 +517,15 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -590,9 +542,9 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="2:30" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -623,7 +575,7 @@
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
     </row>
-    <row r="3" spans="2:30" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -654,89 +606,57 @@
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B5" s="8" t="s">
-        <v>8</v>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:30" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+    </row>
+    <row r="6" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="8" spans="1:30" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:30" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:30" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:30" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B9:F9"/>
+  <mergeCells count="3">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>

</xml_diff>